<commit_message>
Fix: google drive ve anket sonuçları
</commit_message>
<xml_diff>
--- a/Kullanici_Listesi_Tokenli.xlsx
+++ b/Kullanici_Listesi_Tokenli.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hande/anket_uygulama/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A8C4D7-0BF5-D641-B32B-9640A297418E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="760" windowWidth="28840" windowHeight="18260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -604,8 +610,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -676,18 +682,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Köprü" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -725,7 +739,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -759,6 +773,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -793,9 +808,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -968,14 +984,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="72.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -986,7 +1007,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -997,7 +1018,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1008,7 +1029,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1019,7 +1040,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1030,7 +1051,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1041,7 +1062,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1052,7 +1073,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1063,7 +1084,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1074,7 +1095,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1085,7 +1106,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1096,7 +1117,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1107,7 +1128,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1118,7 +1139,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1129,7 +1150,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1140,7 +1161,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1151,7 +1172,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1162,7 +1183,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1173,7 +1194,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1184,7 +1205,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1195,7 +1216,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1206,7 +1227,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1217,7 +1238,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1228,7 +1249,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1239,7 +1260,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1250,7 +1271,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1261,7 +1282,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1272,7 +1293,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -1283,7 +1304,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -1294,7 +1315,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -1305,7 +1326,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -1316,7 +1337,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -1327,7 +1348,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -1338,7 +1359,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -1349,7 +1370,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -1360,7 +1381,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -1371,7 +1392,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -1382,7 +1403,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -1393,7 +1414,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -1404,7 +1425,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -1415,7 +1436,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -1426,7 +1447,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -1437,7 +1458,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>44</v>
       </c>
@@ -1448,7 +1469,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -1459,7 +1480,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -1470,7 +1491,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>47</v>
       </c>
@@ -1481,7 +1502,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>48</v>
       </c>
@@ -1492,7 +1513,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>49</v>
       </c>
@@ -1503,7 +1524,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>50</v>
       </c>
@@ -1514,7 +1535,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>51</v>
       </c>
@@ -1525,7 +1546,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>52</v>
       </c>
@@ -1536,7 +1557,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>53</v>
       </c>
@@ -1547,7 +1568,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>54</v>
       </c>
@@ -1558,7 +1579,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>55</v>
       </c>
@@ -1569,7 +1590,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>56</v>
       </c>
@@ -1580,7 +1601,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>57</v>
       </c>
@@ -1591,7 +1612,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>58</v>
       </c>
@@ -1602,7 +1623,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>59</v>
       </c>
@@ -1613,7 +1634,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>60</v>
       </c>
@@ -1624,7 +1645,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>61</v>
       </c>
@@ -1635,7 +1656,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>62</v>
       </c>
@@ -1646,7 +1667,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>63</v>
       </c>
@@ -1657,7 +1678,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>64</v>
       </c>
@@ -1668,7 +1689,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>65</v>
       </c>
@@ -1679,7 +1700,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>66</v>
       </c>
@@ -1692,70 +1713,70 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
-    <hyperlink ref="C7" r:id="rId6"/>
-    <hyperlink ref="C8" r:id="rId7"/>
-    <hyperlink ref="C9" r:id="rId8"/>
-    <hyperlink ref="C10" r:id="rId9"/>
-    <hyperlink ref="C11" r:id="rId10"/>
-    <hyperlink ref="C12" r:id="rId11"/>
-    <hyperlink ref="C13" r:id="rId12"/>
-    <hyperlink ref="C14" r:id="rId13"/>
-    <hyperlink ref="C15" r:id="rId14"/>
-    <hyperlink ref="C16" r:id="rId15"/>
-    <hyperlink ref="C17" r:id="rId16"/>
-    <hyperlink ref="C18" r:id="rId17"/>
-    <hyperlink ref="C19" r:id="rId18"/>
-    <hyperlink ref="C20" r:id="rId19"/>
-    <hyperlink ref="C21" r:id="rId20"/>
-    <hyperlink ref="C22" r:id="rId21"/>
-    <hyperlink ref="C23" r:id="rId22"/>
-    <hyperlink ref="C24" r:id="rId23"/>
-    <hyperlink ref="C25" r:id="rId24"/>
-    <hyperlink ref="C26" r:id="rId25"/>
-    <hyperlink ref="C27" r:id="rId26"/>
-    <hyperlink ref="C28" r:id="rId27"/>
-    <hyperlink ref="C29" r:id="rId28"/>
-    <hyperlink ref="C30" r:id="rId29"/>
-    <hyperlink ref="C31" r:id="rId30"/>
-    <hyperlink ref="C32" r:id="rId31"/>
-    <hyperlink ref="C33" r:id="rId32"/>
-    <hyperlink ref="C34" r:id="rId33"/>
-    <hyperlink ref="C35" r:id="rId34"/>
-    <hyperlink ref="C36" r:id="rId35"/>
-    <hyperlink ref="C37" r:id="rId36"/>
-    <hyperlink ref="C38" r:id="rId37"/>
-    <hyperlink ref="C39" r:id="rId38"/>
-    <hyperlink ref="C40" r:id="rId39"/>
-    <hyperlink ref="C41" r:id="rId40"/>
-    <hyperlink ref="C42" r:id="rId41"/>
-    <hyperlink ref="C43" r:id="rId42"/>
-    <hyperlink ref="C44" r:id="rId43"/>
-    <hyperlink ref="C45" r:id="rId44"/>
-    <hyperlink ref="C46" r:id="rId45"/>
-    <hyperlink ref="C47" r:id="rId46"/>
-    <hyperlink ref="C48" r:id="rId47"/>
-    <hyperlink ref="C49" r:id="rId48"/>
-    <hyperlink ref="C50" r:id="rId49"/>
-    <hyperlink ref="C51" r:id="rId50"/>
-    <hyperlink ref="C52" r:id="rId51"/>
-    <hyperlink ref="C53" r:id="rId52"/>
-    <hyperlink ref="C54" r:id="rId53"/>
-    <hyperlink ref="C55" r:id="rId54"/>
-    <hyperlink ref="C56" r:id="rId55"/>
-    <hyperlink ref="C57" r:id="rId56"/>
-    <hyperlink ref="C58" r:id="rId57"/>
-    <hyperlink ref="C59" r:id="rId58"/>
-    <hyperlink ref="C60" r:id="rId59"/>
-    <hyperlink ref="C61" r:id="rId60"/>
-    <hyperlink ref="C62" r:id="rId61"/>
-    <hyperlink ref="C63" r:id="rId62"/>
-    <hyperlink ref="C64" r:id="rId63"/>
-    <hyperlink ref="C65" r:id="rId64"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="C13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="C14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="C15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="C16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="C17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="C18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="C19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="C20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="C21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="C22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="C23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="C24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="C25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="C26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="C27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="C28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="C29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="C30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="C31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="C32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="C33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="C34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="C35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="C36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="C37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="C38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="C39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="C40" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="C41" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="C42" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="C43" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="C44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="C45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="C46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="C47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="C48" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="C49" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="C50" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="C51" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="C52" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="C53" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="C54" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="C55" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="C56" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="C57" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="C58" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="C59" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="C60" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="C61" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="C62" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="C63" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="C64" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="C65" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Token listesi güncellendi, bitirenler silindi
</commit_message>
<xml_diff>
--- a/Kullanici_Listesi_Tokenli.xlsx
+++ b/Kullanici_Listesi_Tokenli.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hande/anket_uygulama/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA551E60-5EAD-4441-97CE-83A57BA0590A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A0BE3FD-7F49-4744-846E-5F7026B5152B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10940" yWindow="760" windowWidth="19300" windowHeight="18040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1039,7 +1039,7 @@
   <dimension ref="A1:C70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C4" sqref="C4:C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Güncel token listesi ve kodlar yüklendi
</commit_message>
<xml_diff>
--- a/Kullanici_Listesi_Tokenli.xlsx
+++ b/Kullanici_Listesi_Tokenli.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hande/anket_uygulama/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A0BE3FD-7F49-4744-846E-5F7026B5152B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A755659-D350-BC4C-906B-5E446422E5C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10940" yWindow="760" windowWidth="19300" windowHeight="18040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="145">
   <si>
     <t>Adı Soyadı</t>
   </si>
@@ -223,99 +223,30 @@
     <t>91cb325eaf3c42879347f7f55f0bc7c8</t>
   </si>
   <si>
-    <t>e39a224a9585441fac81cde1256b5df8</t>
-  </si>
-  <si>
-    <t>21c3c9aff73e4896871417b5143b6b7a</t>
-  </si>
-  <si>
     <t>f7a1e1fded0947859b8c3f57d1d6aafe</t>
   </si>
   <si>
-    <t>5703a57f123742929f35780ab3087b35</t>
-  </si>
-  <si>
-    <t>81afec1605d74d0bb35a40f07d2f160f</t>
-  </si>
-  <si>
     <t>0172e0770ce94027823cc6e66033fcf2</t>
   </si>
   <si>
-    <t>4b4fb73f7a9b485a9a9479de1d3322d3</t>
-  </si>
-  <si>
     <t>8a3515f602ae408c947a3ba44faf9c65</t>
   </si>
   <si>
-    <t>54c7d4f2e6994064a3189778cbd887a3</t>
-  </si>
-  <si>
-    <t>590ae7f170e749038a542bd991767c81</t>
-  </si>
-  <si>
-    <t>51e5df0f9f9740a4a4e3a0383e8b00c1</t>
-  </si>
-  <si>
     <t>8bf78ee711594fa586e8d4a1a3d6e271</t>
   </si>
   <si>
-    <t>8e0f8daf72ab4b2eb60f33d2dfb05904</t>
-  </si>
-  <si>
-    <t>926b746df23b407a888a4d14925a291d</t>
-  </si>
-  <si>
     <t>5ff1ba75e27e42a7b42c9a6762870e7c</t>
   </si>
   <si>
-    <t>2bb0b09d4ff84c4eb83127f21ba74dc8</t>
-  </si>
-  <si>
     <t>d123b1568d3f4f8eb61867e74613ffa7</t>
   </si>
   <si>
-    <t>acc19f8f965242e986303d4329081501</t>
-  </si>
-  <si>
     <t>007d4f0b1bd5413995eee774c12f3e40</t>
   </si>
   <si>
-    <t>d356a5d14b87447d96ba13af533d680f</t>
-  </si>
-  <si>
-    <t>b935e17e15ad4af3914ed8a0ca1c398b</t>
-  </si>
-  <si>
-    <t>39ce3bcbdf5545c49039f7ec28a8e2be</t>
-  </si>
-  <si>
-    <t>498412ea51bc47dc9e587fc301424efc</t>
-  </si>
-  <si>
-    <t>6068a6b6323e4e12893d00d234806c38</t>
-  </si>
-  <si>
-    <t>95ac9ca9f8984b658618059a9ddbcffa</t>
-  </si>
-  <si>
-    <t>da92ffd58f9142808a15337146eef908</t>
-  </si>
-  <si>
-    <t>a9e081ac233d45a19ac2842e835cebc8</t>
-  </si>
-  <si>
-    <t>723501f12aa743a9b77010157a6782f1</t>
-  </si>
-  <si>
-    <t>1faa6335d8ef49a1a3f16504cc694121</t>
-  </si>
-  <si>
     <t>a272f6fd889546e1989ce5f194bf428e</t>
   </si>
   <si>
-    <t>6d47ba3ba83348ec9fca5514778c7af3</t>
-  </si>
-  <si>
     <t>abb04885b312419fa43359108bd1b0dc</t>
   </si>
   <si>
@@ -325,189 +256,60 @@
     <t>544d77197e6942118948db0451ac8c30</t>
   </si>
   <si>
-    <t>a234b362525c4a8f82152697f345140b</t>
-  </si>
-  <si>
-    <t>8d17133500a84591be3c6c0333cf93c0</t>
-  </si>
-  <si>
-    <t>f9d948e7989e48bfb3075ae9333ef2b6</t>
-  </si>
-  <si>
     <t>e87daf6cd8c04f97bdda45b9c9e5013e</t>
   </si>
   <si>
     <t>d9f592e1741548228ed1cf738f7d78e1</t>
   </si>
   <si>
-    <t>dcac2c8851474bacb743fa16065c149a</t>
-  </si>
-  <si>
-    <t>383314f3468c4444b9201c6cedf70400</t>
-  </si>
-  <si>
-    <t>e6801ef2b75546fbafc6da99672561c7</t>
-  </si>
-  <si>
     <t>54b5905a609945c183ebe016794f14c4</t>
   </si>
   <si>
-    <t>2c3b9aef15f44505a7417bfd9ad40a8c</t>
-  </si>
-  <si>
     <t>dc42853277554a6a94e692fa32cf3540</t>
   </si>
   <si>
     <t>75ae183bea004a82bfe5f1ca31be16f8</t>
   </si>
   <si>
-    <t>51fc17390e9d451ca832a10382e8bf81</t>
-  </si>
-  <si>
-    <t>20c1211e0cbd498787b559f72db164c7</t>
-  </si>
-  <si>
-    <t>9b94d1aa8c354024991bcfd746565e73</t>
-  </si>
-  <si>
     <t>c7be82fd9dce4eecacf0641f153a283f</t>
   </si>
   <si>
-    <t>7d3d5859d3f44217afe8155327f26a4a</t>
-  </si>
-  <si>
-    <t>15b3bd0b46dd4c54a18ccdc9f7766c48</t>
-  </si>
-  <si>
     <t>058ea380d6f24338b2397a7a3f5a9887</t>
   </si>
   <si>
-    <t>42caeacd304a4b75b38ed0e2ed5af4a8</t>
-  </si>
-  <si>
-    <t>2a31dca07df5424ba1e732598601f250</t>
-  </si>
-  <si>
     <t>7b1bbd9e9a61430aab9d0f8ef0a8e63a</t>
   </si>
   <si>
-    <t>3b3bf91a315344e4a0146c9fb75db9e2</t>
-  </si>
-  <si>
-    <t>16ccb0095d684905adcefb2097ad9d3f</t>
-  </si>
-  <si>
-    <t>afeb73ee07b34421a5c856079b48b292</t>
-  </si>
-  <si>
-    <t>6db2493fd0784fea9e3991f2f0489381</t>
-  </si>
-  <si>
-    <t>596946dc12ce404190d2d750d44c3359</t>
-  </si>
-  <si>
-    <t>a8b2cca4b162461d9f4969945f7446d4</t>
-  </si>
-  <si>
     <t>f136f1903e21eda7d518190678b37c62</t>
   </si>
   <si>
     <t>https://arge-anket-calismasi.streamlit.app/?token=91cb325eaf3c42879347f7f55f0bc7c8</t>
   </si>
   <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=e39a224a9585441fac81cde1256b5df8</t>
-  </si>
-  <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=21c3c9aff73e4896871417b5143b6b7a</t>
-  </si>
-  <si>
     <t>https://arge-anket-calismasi.streamlit.app/?token=f7a1e1fded0947859b8c3f57d1d6aafe</t>
   </si>
   <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=5703a57f123742929f35780ab3087b35</t>
-  </si>
-  <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=81afec1605d74d0bb35a40f07d2f160f</t>
-  </si>
-  <si>
     <t>https://arge-anket-calismasi.streamlit.app/?token=0172e0770ce94027823cc6e66033fcf2</t>
   </si>
   <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=4b4fb73f7a9b485a9a9479de1d3322d3</t>
-  </si>
-  <si>
     <t>https://arge-anket-calismasi.streamlit.app/?token=8a3515f602ae408c947a3ba44faf9c65</t>
   </si>
   <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=54c7d4f2e6994064a3189778cbd887a3</t>
-  </si>
-  <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=590ae7f170e749038a542bd991767c81</t>
-  </si>
-  <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=51e5df0f9f9740a4a4e3a0383e8b00c1</t>
-  </si>
-  <si>
     <t>https://arge-anket-calismasi.streamlit.app/?token=8bf78ee711594fa586e8d4a1a3d6e271</t>
   </si>
   <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=8e0f8daf72ab4b2eb60f33d2dfb05904</t>
-  </si>
-  <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=926b746df23b407a888a4d14925a291d</t>
-  </si>
-  <si>
     <t>https://arge-anket-calismasi.streamlit.app/?token=5ff1ba75e27e42a7b42c9a6762870e7c</t>
   </si>
   <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=2bb0b09d4ff84c4eb83127f21ba74dc8</t>
-  </si>
-  <si>
     <t>https://arge-anket-calismasi.streamlit.app/?token=d123b1568d3f4f8eb61867e74613ffa7</t>
   </si>
   <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=acc19f8f965242e986303d4329081501</t>
-  </si>
-  <si>
     <t>https://arge-anket-calismasi.streamlit.app/?token=007d4f0b1bd5413995eee774c12f3e40</t>
   </si>
   <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=d356a5d14b87447d96ba13af533d680f</t>
-  </si>
-  <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=b935e17e15ad4af3914ed8a0ca1c398b</t>
-  </si>
-  <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=39ce3bcbdf5545c49039f7ec28a8e2be</t>
-  </si>
-  <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=498412ea51bc47dc9e587fc301424efc</t>
-  </si>
-  <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=6068a6b6323e4e12893d00d234806c38</t>
-  </si>
-  <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=95ac9ca9f8984b658618059a9ddbcffa</t>
-  </si>
-  <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=da92ffd58f9142808a15337146eef908</t>
-  </si>
-  <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=a9e081ac233d45a19ac2842e835cebc8</t>
-  </si>
-  <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=723501f12aa743a9b77010157a6782f1</t>
-  </si>
-  <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=1faa6335d8ef49a1a3f16504cc694121</t>
-  </si>
-  <si>
     <t>https://arge-anket-calismasi.streamlit.app/?token=a272f6fd889546e1989ce5f194bf428e</t>
   </si>
   <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=6d47ba3ba83348ec9fca5514778c7af3</t>
-  </si>
-  <si>
     <t>https://arge-anket-calismasi.streamlit.app/?token=abb04885b312419fa43359108bd1b0dc</t>
   </si>
   <si>
@@ -517,90 +319,30 @@
     <t>https://arge-anket-calismasi.streamlit.app/?token=544d77197e6942118948db0451ac8c30</t>
   </si>
   <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=a234b362525c4a8f82152697f345140b</t>
-  </si>
-  <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=8d17133500a84591be3c6c0333cf93c0</t>
-  </si>
-  <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=f9d948e7989e48bfb3075ae9333ef2b6</t>
-  </si>
-  <si>
     <t>https://arge-anket-calismasi.streamlit.app/?token=e87daf6cd8c04f97bdda45b9c9e5013e</t>
   </si>
   <si>
     <t>https://arge-anket-calismasi.streamlit.app/?token=d9f592e1741548228ed1cf738f7d78e1</t>
   </si>
   <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=dcac2c8851474bacb743fa16065c149a</t>
-  </si>
-  <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=383314f3468c4444b9201c6cedf70400</t>
-  </si>
-  <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=e6801ef2b75546fbafc6da99672561c7</t>
-  </si>
-  <si>
     <t>https://arge-anket-calismasi.streamlit.app/?token=54b5905a609945c183ebe016794f14c4</t>
   </si>
   <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=2c3b9aef15f44505a7417bfd9ad40a8c</t>
-  </si>
-  <si>
     <t>https://arge-anket-calismasi.streamlit.app/?token=dc42853277554a6a94e692fa32cf3540</t>
   </si>
   <si>
     <t>https://arge-anket-calismasi.streamlit.app/?token=75ae183bea004a82bfe5f1ca31be16f8</t>
   </si>
   <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=51fc17390e9d451ca832a10382e8bf81</t>
-  </si>
-  <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=20c1211e0cbd498787b559f72db164c7</t>
-  </si>
-  <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=9b94d1aa8c354024991bcfd746565e73</t>
-  </si>
-  <si>
     <t>https://arge-anket-calismasi.streamlit.app/?token=c7be82fd9dce4eecacf0641f153a283f</t>
   </si>
   <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=7d3d5859d3f44217afe8155327f26a4a</t>
-  </si>
-  <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=15b3bd0b46dd4c54a18ccdc9f7766c48</t>
-  </si>
-  <si>
     <t>https://arge-anket-calismasi.streamlit.app/?token=058ea380d6f24338b2397a7a3f5a9887</t>
   </si>
   <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=42caeacd304a4b75b38ed0e2ed5af4a8</t>
-  </si>
-  <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=2a31dca07df5424ba1e732598601f250</t>
-  </si>
-  <si>
     <t>https://arge-anket-calismasi.streamlit.app/?token=7b1bbd9e9a61430aab9d0f8ef0a8e63a</t>
   </si>
   <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=3b3bf91a315344e4a0146c9fb75db9e2</t>
-  </si>
-  <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=16ccb0095d684905adcefb2097ad9d3f</t>
-  </si>
-  <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=afeb73ee07b34421a5c856079b48b292</t>
-  </si>
-  <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=6db2493fd0784fea9e3991f2f0489381</t>
-  </si>
-  <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=596946dc12ce404190d2d750d44c3359</t>
-  </si>
-  <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=a8b2cca4b162461d9f4969945f7446d4</t>
-  </si>
-  <si>
     <t>https://arge-anket-calismasi.streamlit.app/?token=f136f1903e21eda7d518190678b37c62</t>
   </si>
   <si>
@@ -610,12 +352,6 @@
     <t>TEST USER2</t>
   </si>
   <si>
-    <t>c3c547e2aaef4ea4a5b874ef6de2a67f</t>
-  </si>
-  <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=c3c547e2aaef4ea4a5b874ef6de2a67f</t>
-  </si>
-  <si>
     <t>BURHAN TOKOVA</t>
   </si>
   <si>
@@ -628,35 +364,104 @@
     <t>OSMAN ONUR GÖKAY</t>
   </si>
   <si>
-    <t>ac4f39ea13f8481189bd4782f47f203e</t>
-  </si>
-  <si>
-    <t>bc71924f72334e27a4cc38c05c77d9a1</t>
-  </si>
-  <si>
-    <t>e23190cbdf374d128c4307fdc9841b42</t>
-  </si>
-  <si>
     <t>d82b71e6fef84a92aef5e8d6dbd6d8be</t>
   </si>
   <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=ac4f39ea13f8481189bd4782f47f203e</t>
-  </si>
-  <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=bc71924f72334e27a4cc38c05c77d9a1</t>
-  </si>
-  <si>
-    <t>https://arge-anket-calismasi.streamlit.app/?token=e23190cbdf374d128c4307fdc9841b42</t>
-  </si>
-  <si>
     <t>https://arge-anket-calismasi.streamlit.app/?token=d82b71e6fef84a92aef5e8d6dbd6d8be</t>
+  </si>
+  <si>
+    <t>vsfsd</t>
+  </si>
+  <si>
+    <t>vdss</t>
+  </si>
+  <si>
+    <t>vsv</t>
+  </si>
+  <si>
+    <t>svdv</t>
+  </si>
+  <si>
+    <t>vssv</t>
+  </si>
+  <si>
+    <t>svds</t>
+  </si>
+  <si>
+    <t>sdv</t>
+  </si>
+  <si>
+    <t>sv</t>
+  </si>
+  <si>
+    <t>vvdsv</t>
+  </si>
+  <si>
+    <t>sdvs</t>
+  </si>
+  <si>
+    <t>svd</t>
+  </si>
+  <si>
+    <t>vsd</t>
+  </si>
+  <si>
+    <t>dfsd</t>
+  </si>
+  <si>
+    <t>svsv</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>dv</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>sf</t>
+  </si>
+  <si>
+    <t>sdfs</t>
+  </si>
+  <si>
+    <t>fsdfs</t>
+  </si>
+  <si>
+    <t>dsfs</t>
+  </si>
+  <si>
+    <t>fsds</t>
+  </si>
+  <si>
+    <t>ff</t>
+  </si>
+  <si>
+    <t>sfs</t>
+  </si>
+  <si>
+    <t>sdfsd</t>
+  </si>
+  <si>
+    <t>sfsdfs</t>
+  </si>
+  <si>
+    <t>fsfs</t>
+  </si>
+  <si>
+    <t>sdfsdf</t>
+  </si>
+  <si>
+    <t>sfssfsfdsd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -681,6 +486,21 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -725,12 +545,15 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Köprü" xfId="1" builtinId="8"/>
@@ -1039,13 +862,13 @@
   <dimension ref="A1:C70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C70"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.33203125" customWidth="1"/>
+    <col min="2" max="2" width="33.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="72.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1062,431 +885,377 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>194</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>129</v>
+        <v>86</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>193</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>195</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
         <v>66</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>130</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>196</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>197</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>131</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>132</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>133</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>134</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>135</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>136</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>73</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>137</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>138</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>139</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>140</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>198</v>
+      <c r="A15" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="B15" t="s">
-        <v>202</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>206</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>141</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>142</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>79</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>143</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>80</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>144</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>145</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>199</v>
+      <c r="A21" s="3" t="s">
+        <v>111</v>
       </c>
       <c r="B21" t="s">
-        <v>203</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>207</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="C21" s="2"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>146</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="C22" s="2"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>147</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="A24" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>84</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>148</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="C24" s="2"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="A25" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>149</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="A26" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>86</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>150</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="C26" s="2"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="A27" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>87</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>151</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="C27" s="2"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="A28" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>88</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>152</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="C28" s="2"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="A29" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>89</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>153</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="C29" s="2"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="A30" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>90</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>154</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="C30" s="2"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="A31" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>91</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>155</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="C31" s="2"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="A32" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>92</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>156</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="C32" s="2"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="A33" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>93</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>157</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="C33" s="2"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="A34" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>94</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>158</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="C34" s="2"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="A35" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>95</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>159</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="C35" s="2"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>160</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="A37" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>97</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>161</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="C37" s="2"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>162</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>200</v>
+      <c r="A39" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="B39" t="s">
-        <v>204</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>208</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="C39" s="2"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>36</v>
       </c>
       <c r="B40" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>163</v>
+        <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -1494,54 +1263,48 @@
         <v>37</v>
       </c>
       <c r="B41" t="s">
-        <v>100</v>
+        <v>77</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>164</v>
+        <v>98</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="A42" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B42" t="s">
-        <v>101</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>165</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="C42" s="2"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="A43" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B43" t="s">
-        <v>102</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>166</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="C43" s="2"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="A44" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B44" t="s">
-        <v>103</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>167</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="C44" s="2"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>41</v>
       </c>
       <c r="B45" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>168</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -1549,76 +1312,68 @@
         <v>42</v>
       </c>
       <c r="B46" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>169</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+      <c r="A47" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B47" t="s">
-        <v>106</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>170</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="C47" s="2"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+      <c r="A48" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B48" t="s">
-        <v>107</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>171</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="C48" s="2"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="A49" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B49" t="s">
-        <v>108</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>172</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="C49" s="2"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+      <c r="A50" s="5" t="s">
         <v>46</v>
       </c>
       <c r="B50" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>173</v>
+        <v>101</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+      <c r="A51" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B51" t="s">
-        <v>110</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>174</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="C51" s="2"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>48</v>
       </c>
       <c r="B52" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>175</v>
+        <v>102</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -1626,54 +1381,48 @@
         <v>49</v>
       </c>
       <c r="B53" t="s">
-        <v>112</v>
+        <v>82</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>176</v>
+        <v>103</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+      <c r="A54" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B54" t="s">
-        <v>113</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>177</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="C54" s="2"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+      <c r="A55" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B55" t="s">
-        <v>114</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>178</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="C55" s="2"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+      <c r="A56" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B56" t="s">
-        <v>115</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>179</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="C56" s="2"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>201</v>
+        <v>113</v>
       </c>
       <c r="B57" t="s">
-        <v>205</v>
+        <v>114</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>209</v>
+        <v>115</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -1681,216 +1430,149 @@
         <v>53</v>
       </c>
       <c r="B58" t="s">
-        <v>116</v>
+        <v>83</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>180</v>
+        <v>104</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+      <c r="A59" s="3" t="s">
         <v>54</v>
       </c>
       <c r="B59" t="s">
-        <v>117</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>181</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="C59" s="2"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+      <c r="A60" s="3" t="s">
         <v>55</v>
       </c>
       <c r="B60" t="s">
-        <v>118</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>182</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="C60" s="2"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>56</v>
       </c>
       <c r="B61" t="s">
-        <v>119</v>
+        <v>84</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>183</v>
+        <v>105</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+      <c r="A62" s="3" t="s">
         <v>57</v>
       </c>
       <c r="B62" t="s">
-        <v>120</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>184</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="C62" s="2"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+      <c r="A63" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B63" t="s">
-        <v>121</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>185</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="C63" s="2"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>59</v>
       </c>
       <c r="B64" t="s">
-        <v>122</v>
+        <v>85</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>186</v>
+        <v>106</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+      <c r="A65" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B65" t="s">
-        <v>123</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>187</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="C65" s="2"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+      <c r="A66" s="3" t="s">
         <v>61</v>
       </c>
       <c r="B66" t="s">
-        <v>124</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>188</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="C66" s="2"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
+      <c r="A67" s="3" t="s">
         <v>62</v>
       </c>
       <c r="B67" t="s">
-        <v>125</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>189</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="C67" s="2"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
+      <c r="A68" s="3" t="s">
         <v>63</v>
       </c>
       <c r="B68" t="s">
-        <v>126</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>190</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="C68" s="2"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+      <c r="A69" s="3" t="s">
         <v>64</v>
       </c>
       <c r="B69" t="s">
-        <v>127</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>191</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="C69" s="2"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
+      <c r="A70" s="3" t="s">
         <v>65</v>
       </c>
       <c r="B70" t="s">
-        <v>128</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>192</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="C70" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C7" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="C9" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="C10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="C11" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="C12" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="C13" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="C14" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="C16" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="C17" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="C18" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="C19" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="C20" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="C22" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="C23" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="C24" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="C25" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="C26" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="C27" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="C28" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="C29" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="C30" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="C31" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="C32" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="C33" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="C34" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="C35" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="C36" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="C37" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="C38" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="C40" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="C41" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="C42" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="C43" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="C44" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="C45" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="C46" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="C47" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="C48" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="C49" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="C50" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="C51" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="C52" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="C53" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="C54" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="C55" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="C56" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="C58" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="C59" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="C60" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="C61" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="C62" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="C63" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="C64" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="C65" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="C66" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="C67" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="C68" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="C69" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="C70" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="C2" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="C4" r:id="rId65" xr:uid="{B7AA4B0B-2571-EB4A-BE15-AE02F7698588}"/>
-    <hyperlink ref="C57" r:id="rId66" xr:uid="{0ED140D5-BBD8-4B4C-9C17-72D7C924E22B}"/>
-    <hyperlink ref="C39" r:id="rId67" xr:uid="{E9529E13-8347-7940-AB43-B739D2DBE387}"/>
-    <hyperlink ref="C21" r:id="rId68" xr:uid="{5B2731C9-E8A9-8544-81B6-5F39A04B7A99}"/>
-    <hyperlink ref="C15" r:id="rId69" xr:uid="{0AB330E8-3505-7349-8F27-4428D6949D05}"/>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{A67EEAC5-8112-9244-88C3-2C5C629F96D6}"/>
+    <hyperlink ref="C7" r:id="rId2" xr:uid="{E446AE1B-6249-644F-BD18-2849BD638089}"/>
+    <hyperlink ref="C10" r:id="rId3" xr:uid="{843159A5-000D-F744-A893-7FE97A91E0F1}"/>
+    <hyperlink ref="C12" r:id="rId4" xr:uid="{975CCF1C-E1D2-9841-A10C-915BF99D679F}"/>
+    <hyperlink ref="C17" r:id="rId5" xr:uid="{A1A64825-965A-6843-9563-0FC8D0D76529}"/>
+    <hyperlink ref="C20" r:id="rId6" xr:uid="{C1166E92-E019-074D-AD41-9F97C42D8199}"/>
+    <hyperlink ref="C23" r:id="rId7" xr:uid="{3E98DE70-676B-CB41-8672-01146747D412}"/>
+    <hyperlink ref="C25" r:id="rId8" xr:uid="{4CC75A98-3D41-434D-9588-DA6E0C5A43A5}"/>
+    <hyperlink ref="C36" r:id="rId9" xr:uid="{69F16A78-2739-C24D-9958-FC59D59F61C2}"/>
+    <hyperlink ref="C38" r:id="rId10" xr:uid="{0C119441-BAC7-6B47-B5A3-1DD74B0F2558}"/>
+    <hyperlink ref="C40" r:id="rId11" xr:uid="{BFFA992F-755D-274A-B8E9-D4DF588A88FC}"/>
+    <hyperlink ref="C41" r:id="rId12" xr:uid="{ED531228-4246-3846-976A-1894E20C89E1}"/>
+    <hyperlink ref="C45" r:id="rId13" xr:uid="{2049E17F-5355-7445-B537-FAFDD78385DC}"/>
+    <hyperlink ref="C46" r:id="rId14" xr:uid="{DCCE041B-4C14-DC4C-8126-3D1964C0FC99}"/>
+    <hyperlink ref="C50" r:id="rId15" xr:uid="{120E8DF7-5AB0-F34D-A9C4-71D6BB290A21}"/>
+    <hyperlink ref="C52" r:id="rId16" xr:uid="{A432285C-4DC6-C448-A3A0-4752C334A7A5}"/>
+    <hyperlink ref="C53" r:id="rId17" xr:uid="{2AAA8C30-8066-0143-B381-DC6576CF880B}"/>
+    <hyperlink ref="C58" r:id="rId18" xr:uid="{7F79CC8F-B0D1-C14B-9B4B-DA476902EA98}"/>
+    <hyperlink ref="C61" r:id="rId19" xr:uid="{844CA0EE-2DE2-824F-8094-0EF96C5A2362}"/>
+    <hyperlink ref="C64" r:id="rId20" xr:uid="{594315A8-BCAF-6F44-8BC8-9BB8EA5CB8DE}"/>
+    <hyperlink ref="C2" r:id="rId21" xr:uid="{45F0A614-EBB5-064C-968E-3A819767C16B}"/>
+    <hyperlink ref="C57" r:id="rId22" xr:uid="{BE9D71A9-CAB0-3C4B-9483-FC17FFF420F4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>